<commit_message>
Streamlined to reduce calculations
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v5.xlsx
+++ b/Projects/CCBOTTLERSUS/CMA_SOUTHWEST/Data/Southwest CMA Compliance Template_v5.xlsx
@@ -26,375 +26,375 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="123">
-  <si>
-    <t>KPI name</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>scene types</t>
-  </si>
-  <si>
-    <t>template group</t>
-  </si>
-  <si>
-    <t>program (Additional Attribute 3)</t>
-  </si>
-  <si>
-    <t>Sparkling</t>
-  </si>
-  <si>
-    <t>SOS</t>
-  </si>
-  <si>
-    <t>Cold</t>
-  </si>
-  <si>
-    <t>Club Coke Chill,Club Coke Gold,Club Coke Silver,NTBA</t>
-  </si>
-  <si>
-    <t>Still</t>
-  </si>
-  <si>
-    <t>Club Coke Chill,Club Coke Gold,Club Coke Silver</t>
-  </si>
-  <si>
-    <t>Energy KO</t>
-  </si>
-  <si>
-    <t>Energy Monster</t>
-  </si>
-  <si>
-    <t>Coffee/Dairy</t>
-  </si>
-  <si>
-    <t>number of shelves</t>
-  </si>
-  <si>
-    <t>Protein</t>
-  </si>
-  <si>
-    <t>Enhanced Water</t>
-  </si>
-  <si>
-    <t>Powerade Bonus</t>
-  </si>
-  <si>
-    <t>number of shelves bonus</t>
-  </si>
-  <si>
-    <t>Smartwater Bonus</t>
-  </si>
-  <si>
-    <t>Gold Peak Tea Bonus</t>
-  </si>
-  <si>
-    <t>Impulse Zone Cooler</t>
-  </si>
-  <si>
-    <t>1:1 ratio</t>
-  </si>
-  <si>
-    <t>Impulse Zone Coolers</t>
-  </si>
-  <si>
-    <t>Juice</t>
-  </si>
-  <si>
-    <t>SOS - Target</t>
-  </si>
-  <si>
-    <t>NTBA</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>Isotonics</t>
-  </si>
-  <si>
-    <t>Premium/Enchanced Water</t>
-  </si>
-  <si>
-    <t>Tea</t>
-  </si>
-  <si>
-    <t>Diet Coke Sleek Can 12 oz</t>
-  </si>
-  <si>
-    <t>Facings NTBA</t>
-  </si>
-  <si>
-    <t>Cold Vault &amp; Coolers with Doors (Outside of Checkout Area)</t>
-  </si>
-  <si>
-    <t>Monster Mutant</t>
-  </si>
-  <si>
-    <t>Topo Chico</t>
-  </si>
-  <si>
-    <t>Vitamin Water Active</t>
-  </si>
-  <si>
-    <t>Monster Hydro</t>
-  </si>
-  <si>
-    <t>Huberts</t>
-  </si>
-  <si>
-    <t>McCafe</t>
-  </si>
-  <si>
-    <t>Monster Coffee</t>
-  </si>
-  <si>
-    <t>KPI Name</t>
-  </si>
-  <si>
-    <t>product_ean_code</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>Visible</t>
-  </si>
-  <si>
-    <t>7613035738539, 7613035738119, 50189779, 50251797, 7613035220065, 7613034954459, 3800020415009, 7613035058347, 7613035052024, 7613034872630, 50251414, 761303495928</t>
-  </si>
-  <si>
-    <t>numerator param 1</t>
-  </si>
-  <si>
-    <t>numerator value 1</t>
-  </si>
-  <si>
-    <t>numerator param 2</t>
-  </si>
-  <si>
-    <t>numerator value 2</t>
-  </si>
-  <si>
-    <t>numerator param 3</t>
-  </si>
-  <si>
-    <t>numerator value 3</t>
-  </si>
-  <si>
-    <t>denominator param 1</t>
-  </si>
-  <si>
-    <t>denominator value 1</t>
-  </si>
-  <si>
-    <t>denominator param 2</t>
-  </si>
-  <si>
-    <t>denominator value 2</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>Southwest Deliver</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>att4</t>
-  </si>
-  <si>
-    <t>EnergyKO</t>
-  </si>
-  <si>
-    <t>brand_name</t>
-  </si>
-  <si>
-    <t>NOS ENERGY,FULL THROTTLE</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>MONSTER ENERGY</t>
-  </si>
-  <si>
-    <t>Isotonic</t>
-  </si>
-  <si>
-    <t>sub_category</t>
-  </si>
-  <si>
-    <t>Enhanced</t>
-  </si>
-  <si>
-    <t>Param 1</t>
-  </si>
-  <si>
-    <t>Value 1</t>
-  </si>
-  <si>
-    <t>Param 2</t>
-  </si>
-  <si>
-    <t>Value 2</t>
-  </si>
-  <si>
-    <t>Param 3</t>
-  </si>
-  <si>
-    <t>Value 3</t>
-  </si>
-  <si>
-    <t>Dairy</t>
-  </si>
-  <si>
-    <t>Coffee</t>
-  </si>
-  <si>
-    <t>SHELF STABLE PROTEIN</t>
-  </si>
-  <si>
-    <t>Client Subcategory Name</t>
-  </si>
-  <si>
-    <t>POWERADE</t>
-  </si>
-  <si>
-    <t>SMARTWATER</t>
-  </si>
-  <si>
-    <t>SMARTWATER SPARKLING</t>
-  </si>
-  <si>
-    <t>GOLD PEAK TEA</t>
-  </si>
-  <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>program</t>
-  </si>
-  <si>
-    <t>Store Type</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>lower limit</t>
-  </si>
-  <si>
-    <t>upper limit</t>
-  </si>
-  <si>
-    <t>SOUTHWEST</t>
-  </si>
-  <si>
-    <t>Club Coke Silver</t>
-  </si>
-  <si>
-    <t>SOS - Range</t>
-  </si>
-  <si>
-    <t>45% - 65%</t>
-  </si>
-  <si>
-    <t>1.5 Shelf</t>
-  </si>
-  <si>
-    <t>1 Shelf</t>
-  </si>
-  <si>
-    <t>.5 Shelf</t>
-  </si>
-  <si>
-    <t>.5 Shelf, 1 Shelf, 2 Shelf, 3 shelf, full door</t>
-  </si>
-  <si>
-    <t>.5 Shelf, 1 Shelf, 2 Shelf</t>
-  </si>
-  <si>
-    <t>1 Shelf, 2 Shelf, 3 shelf</t>
-  </si>
-  <si>
-    <t>1:1 ratio with competition</t>
-  </si>
-  <si>
-    <t>2 door CSD</t>
-  </si>
-  <si>
-    <t>3 door CSD</t>
-  </si>
-  <si>
-    <t>3 door still</t>
-  </si>
-  <si>
-    <t>4 door still</t>
-  </si>
-  <si>
-    <t>5 door still</t>
-  </si>
-  <si>
-    <t>6 door still</t>
-  </si>
-  <si>
-    <t>7 door still</t>
-  </si>
-  <si>
-    <t>8 door still</t>
-  </si>
-  <si>
-    <t>COKE DT</t>
-  </si>
-  <si>
-    <t>att3</t>
-  </si>
-  <si>
-    <t>12oz Can Single</t>
-  </si>
-  <si>
-    <t>product_name</t>
-  </si>
-  <si>
-    <t>Monster Energy Mutant Green,Monster Energy Mutant Red,Monster Mutant Super Soda White Lightning Zero Sugar 20 fl oz</t>
-  </si>
-  <si>
-    <t>TOPO CHICO</t>
-  </si>
-  <si>
-    <t>Vitamin Water Active Pump It 15.2 FL OZ PET,Vitamin Water Active Werk It 15.2 FL OZ PET,Vitamin Water Active Move It 15.2 FL OZ PET</t>
-  </si>
-  <si>
-    <t>MONSTER HYDRO Tropical Thunder 12/25.4oz,MONSTER HYDRO Purple Passion 12/25.4oz,MONSTER HYDRO Blue Ice 12/25.4oz,MONSTER HYDRO Zero Sugar 12/25.4oz</t>
-  </si>
-  <si>
-    <t>Hubert's</t>
-  </si>
-  <si>
-    <t>MC CAFE</t>
-  </si>
-  <si>
-    <t>152687 11Z CN 4P JAVA MON MN BN,145106 15Z CN 12LS JAVA MON KONA CAPP,Monster Java Loca Moca Coffee Energy Drink 15oz,Monster Energy Java Kona Blend 15oz,Monster Energy Java Vanilla Light 15oz,Monster Energy Java Salted Caramel 15oz,Monster Energy Java Monster Loca Mocha 4pk/11oz</t>
-  </si>
-  <si>
-    <t>Monster Cafe?</t>
-  </si>
-  <si>
-    <t>MONSTER Caffe Mocha 13.7 OZ Glass,MONSTER Caffe Vanilla 13.7 OZ Glass,MONSTER Caffe Salted Caramel 13.7 OZ Glass</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="123">
+  <si>
+    <t xml:space="preserve">KPI name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">program (Additional Attribute 3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sparkling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club Coke Chill,Club Coke Gold,Club Coke Silver,NTBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Still</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club Coke Chill,Club Coke Gold,Club Coke Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy KO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Monster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coffee/Dairy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of shelves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enhanced Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powerade Bonus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of shelves bonus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Smartwater Bonus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gold Peak Tea Bonus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulse Zone Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:1 ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impulse Zone Coolers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS - Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isotonics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Premium/Enchanced Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diet Coke Sleek Can 12 oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facings NTBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cold Vault &amp; Coolers with Doors (Outside of Checkout Area)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Mutant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Topo Chico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin Water Active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Hydro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huberts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McCafe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_ean_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7613035738539, 7613035738119, 50189779, 50251797, 7613035220065, 7613034954459, 3800020415009, 7613035058347, 7613035052024, 7613034872630, 50251414, 761303495928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator param 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numerator value 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominator value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southwest Deliver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">att4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EnergyKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOS ENERGY,FULL THROTTLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONSTER ENERGY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isotonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub_category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enhanced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Param 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Param 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Param 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dairy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHELF STABLE PROTEIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Subcategory Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POWERADE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMARTWATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMARTWATER SPARKLING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOLD PEAK TEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOUTHWEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Club Coke Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS - Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45% - 65%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.5 Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.5 Shelf, 1 Shelf, 2 Shelf, 3 shelf, full door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.5 Shelf, 1 Shelf, 2 Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Shelf, 2 Shelf, 3 shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:1 ratio with competition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 door CSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 door CSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 door still</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 door still</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 door still</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 door still</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 door still</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 door still</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COKE DT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">att3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12oz Can Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Energy Mutant Green,Monster Energy Mutant Red,Monster Mutant Super Soda White Lightning Zero Sugar 20 fl oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOPO CHICO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin Water Active Pump It 15.2 FL OZ PET,Vitamin Water Active Werk It 15.2 FL OZ PET,Vitamin Water Active Move It 15.2 FL OZ PET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONSTER HYDRO Tropical Thunder 12/25.4oz,MONSTER HYDRO Purple Passion 12/25.4oz,MONSTER HYDRO Blue Ice 12/25.4oz,MONSTER HYDRO Zero Sugar 12/25.4oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hubert's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC CAFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">152687 11Z CN 4P JAVA MON MN BN,145106 15Z CN 12LS JAVA MON KONA CAPP,Monster Java Loca Moca Coffee Energy Drink 15oz,Monster Energy Java Kona Blend 15oz,Monster Energy Java Vanilla Light 15oz,Monster Energy Java Salted Caramel 15oz,Monster Energy Java Monster Loca Mocha 4pk/11oz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Cafe?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONSTER Caffe Mocha 13.7 OZ Glass,MONSTER Caffe Vanilla 13.7 OZ Glass,MONSTER Caffe Salted Caramel 13.7 OZ Glass</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="0.00%"/>
@@ -528,7 +528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -555,13 +555,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -671,7 +664,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -780,8 +773,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -789,10 +782,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -800,15 +789,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -816,15 +805,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -832,15 +821,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -928,17 +917,17 @@
   </sheetPr>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.8825910931174"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.3117408906883"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1321,7 +1310,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="43.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="43.919028340081"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="6" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="6" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="7" width="9.10526315789474"/>
@@ -1368,24 +1357,24 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.5991902834008"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1665,16 +1654,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
@@ -1847,7 +1836,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1897,11 +1886,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1174089068826"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.5587044534413"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="35.9919028340081"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.46153846153846"/>
@@ -2267,358 +2256,344 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5303643724696"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.46153846153846"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
       <c r="G1" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>102</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="N2" s="30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" s="32" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="33"/>
+    </row>
+    <row r="3" customFormat="false" ht="49" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="36" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="37"/>
+    </row>
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="32" t="n">
+      <c r="C4" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="35"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="33" t="n">
+      <c r="L4" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="34"/>
-    </row>
-    <row r="4" customFormat="false" ht="49" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="M4" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" s="37" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" s="37" t="n">
+      <c r="C5" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="38"/>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="L5" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="M5" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="N5" s="38" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="36" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" s="36" t="n">
+        <v>3</v>
+      </c>
+      <c r="N5" s="37" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="37" t="n">
+      <c r="C6" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="35"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="L6" s="37" t="n">
+      <c r="M6" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="M6" s="37" t="n">
+      <c r="N6" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="N6" s="38" t="n">
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="35"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="L7" s="36" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="L7" s="37" t="n">
+      <c r="M7" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="M7" s="37" t="n">
+      <c r="N7" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="N7" s="38" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37" t="n">
+      <c r="C8" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="35"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="N8" s="37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="89" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="39"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="37" t="n">
+      <c r="J9" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="K8" s="37" t="n">
+      <c r="K9" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="L8" s="37" t="n">
+      <c r="L9" s="40" t="n">
+        <v>2</v>
+      </c>
+      <c r="M9" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="M8" s="37" t="n">
+      <c r="N9" s="41" t="n">
         <v>3</v>
       </c>
-      <c r="N8" s="38" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="M9" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="N9" s="38" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="89" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>40</v>
+    </row>
+    <row r="10" customFormat="false" ht="49" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="41" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="41" t="n">
-        <v>2</v>
-      </c>
-      <c r="L10" s="41" t="n">
-        <v>2</v>
-      </c>
-      <c r="M10" s="41" t="n">
-        <v>3</v>
-      </c>
-      <c r="N10" s="42" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="49" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="43" t="s">
+      <c r="C10" s="42" t="s">
         <v>122</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G1:N1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" display="TOPO CHICO"/>
+    <hyperlink ref="C4" r:id="rId1" display="TOPO CHICO"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>